<commit_message>
atualização do texto do email
</commit_message>
<xml_diff>
--- a/fiis.xlsx
+++ b/fiis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://komatsuforest-my.sharepoint.com/personal/ramon_lara_komatsuforest_com/Documents/Área de Trabalho/Ramon/Fundos_Imobiliarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_82EC7DD58F79A8D366075C52F37BD2728A4AA99B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{584A5CB6-0A3B-452A-87A0-F70B786A1703}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_82EC7DD58F79A8D366075C52F37BD2728A4AA99B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8C13F8D-95DD-4523-BE86-25118161B844}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2339,8 +2339,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O406"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O72"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2436,7 +2436,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>67</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>107</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>108</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>116</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>118</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>119</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>120</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>124</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>125</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>127</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>128</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>130</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>132</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>133</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>136</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>137</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>139</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>140</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>142</v>
       </c>
@@ -5915,7 +5915,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>144</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>145</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>147</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>148</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>152</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>153</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>157</v>
       </c>
@@ -6370,7 +6370,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>159</v>
       </c>
@@ -6417,7 +6417,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>161</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>163</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>166</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>169</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>172</v>
       </c>
@@ -6825,7 +6825,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>174</v>
       </c>
@@ -6872,7 +6872,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>176</v>
       </c>
@@ -6919,7 +6919,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>178</v>
       </c>
@@ -7010,7 +7010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>181</v>
       </c>
@@ -7057,7 +7057,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>183</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>185</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>187</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>190</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>193</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>197</v>
       </c>
@@ -7609,7 +7609,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>203</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>204</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>206</v>
       </c>
@@ -7747,7 +7747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>208</v>
       </c>
@@ -7794,7 +7794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>210</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>212</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>215</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>217</v>
       </c>
@@ -8026,7 +8026,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>219</v>
       </c>
@@ -8120,7 +8120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>223</v>
       </c>
@@ -8167,7 +8167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>225</v>
       </c>
@@ -8211,7 +8211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>226</v>
       </c>
@@ -8255,7 +8255,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>227</v>
       </c>
@@ -8299,7 +8299,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>228</v>
       </c>
@@ -8343,7 +8343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>229</v>
       </c>
@@ -8390,7 +8390,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>231</v>
       </c>
@@ -8484,7 +8484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="135" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>235</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>236</v>
       </c>
@@ -8619,7 +8619,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="138" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>239</v>
       </c>
@@ -8666,7 +8666,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>241</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>243</v>
       </c>
@@ -8760,7 +8760,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="141" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>245</v>
       </c>
@@ -8851,7 +8851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="143" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>248</v>
       </c>
@@ -8942,7 +8942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>251</v>
       </c>
@@ -8986,7 +8986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="146" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>252</v>
       </c>
@@ -9033,7 +9033,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="147" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>255</v>
       </c>
@@ -9121,7 +9121,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>257</v>
       </c>
@@ -9209,7 +9209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="151" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>259</v>
       </c>
@@ -9300,7 +9300,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>262</v>
       </c>
@@ -9344,7 +9344,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>263</v>
       </c>
@@ -9388,7 +9388,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="155" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>264</v>
       </c>
@@ -9482,7 +9482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>268</v>
       </c>
@@ -9529,7 +9529,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>270</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>274</v>
       </c>
@@ -9670,7 +9670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>276</v>
       </c>
@@ -9717,7 +9717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>277</v>
       </c>
@@ -9764,7 +9764,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>279</v>
       </c>
@@ -9808,7 +9808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>280</v>
       </c>
@@ -9855,7 +9855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>282</v>
       </c>
@@ -9899,7 +9899,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>283</v>
       </c>
@@ -9943,7 +9943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>284</v>
       </c>
@@ -9987,7 +9987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>285</v>
       </c>
@@ -10034,7 +10034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>287</v>
       </c>
@@ -10128,7 +10128,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>291</v>
       </c>
@@ -10175,7 +10175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>294</v>
       </c>
@@ -10222,7 +10222,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>296</v>
       </c>
@@ -10269,7 +10269,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>298</v>
       </c>
@@ -10360,7 +10360,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="176" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>301</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="177" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>302</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>303</v>
       </c>
@@ -10580,7 +10580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="181" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>306</v>
       </c>
@@ -10624,7 +10624,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="182" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>307</v>
       </c>
@@ -10668,7 +10668,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="183" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>308</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="185" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>310</v>
       </c>
@@ -10800,7 +10800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="186" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>311</v>
       </c>
@@ -10891,7 +10891,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>314</v>
       </c>
@@ -10938,7 +10938,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>316</v>
       </c>
@@ -11026,7 +11026,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="191" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>318</v>
       </c>
@@ -11070,7 +11070,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="192" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>319</v>
       </c>
@@ -11117,7 +11117,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="193" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>321</v>
       </c>
@@ -11161,7 +11161,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="194" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>322</v>
       </c>
@@ -11208,7 +11208,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="195" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>324</v>
       </c>
@@ -11296,7 +11296,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="197" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>326</v>
       </c>
@@ -11340,7 +11340,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="198" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>327</v>
       </c>
@@ -11384,7 +11384,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="199" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>328</v>
       </c>
@@ -11428,7 +11428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="200" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>329</v>
       </c>
@@ -11516,7 +11516,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="202" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>331</v>
       </c>
@@ -11604,7 +11604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="204" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>333</v>
       </c>
@@ -11648,7 +11648,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="205" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>334</v>
       </c>
@@ -11692,7 +11692,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="206" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>335</v>
       </c>
@@ -11739,7 +11739,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="207" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>337</v>
       </c>
@@ -11783,7 +11783,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="208" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>338</v>
       </c>
@@ -11830,7 +11830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="209" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>340</v>
       </c>
@@ -11924,7 +11924,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="211" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>344</v>
       </c>
@@ -11971,7 +11971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="212" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>346</v>
       </c>
@@ -12106,7 +12106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="215" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>350</v>
       </c>
@@ -12150,7 +12150,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="216" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>351</v>
       </c>
@@ -12197,7 +12197,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="217" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>353</v>
       </c>
@@ -12244,7 +12244,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="218" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>355</v>
       </c>
@@ -12291,7 +12291,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="219" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>357</v>
       </c>
@@ -12335,7 +12335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="220" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>358</v>
       </c>
@@ -12379,7 +12379,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="221" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>359</v>
       </c>
@@ -12426,7 +12426,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="222" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>361</v>
       </c>
@@ -12473,7 +12473,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="223" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>363</v>
       </c>
@@ -12517,7 +12517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="224" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>364</v>
       </c>
@@ -12605,7 +12605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="226" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>366</v>
       </c>
@@ -12649,7 +12649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="227" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>367</v>
       </c>
@@ -12693,7 +12693,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="228" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>368</v>
       </c>
@@ -12740,7 +12740,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="229" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>370</v>
       </c>
@@ -12784,7 +12784,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="230" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>371</v>
       </c>
@@ -12828,7 +12828,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="231" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>372</v>
       </c>
@@ -12919,7 +12919,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="233" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>375</v>
       </c>
@@ -12966,7 +12966,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="234" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>377</v>
       </c>
@@ -13010,7 +13010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="235" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>378</v>
       </c>
@@ -13101,7 +13101,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="237" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>381</v>
       </c>
@@ -13145,7 +13145,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="238" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>382</v>
       </c>
@@ -13189,7 +13189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="239" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>383</v>
       </c>
@@ -13233,7 +13233,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="240" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>384</v>
       </c>
@@ -13277,7 +13277,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="241" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>385</v>
       </c>
@@ -13371,7 +13371,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="243" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>389</v>
       </c>
@@ -13415,7 +13415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="244" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>390</v>
       </c>
@@ -13462,7 +13462,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="245" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>392</v>
       </c>
@@ -13553,7 +13553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="247" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>395</v>
       </c>
@@ -13597,7 +13597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="248" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>396</v>
       </c>
@@ -13644,7 +13644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="249" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>398</v>
       </c>
@@ -13688,7 +13688,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="250" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>399</v>
       </c>
@@ -13735,7 +13735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="251" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>401</v>
       </c>
@@ -13779,7 +13779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="252" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>402</v>
       </c>
@@ -13823,7 +13823,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="253" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>403</v>
       </c>
@@ -13870,7 +13870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="254" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>405</v>
       </c>
@@ -13917,7 +13917,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="255" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>407</v>
       </c>
@@ -13964,7 +13964,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="256" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>409</v>
       </c>
@@ -14058,7 +14058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="258" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>412</v>
       </c>
@@ -14102,7 +14102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="259" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>413</v>
       </c>
@@ -14146,7 +14146,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="260" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>414</v>
       </c>
@@ -14190,7 +14190,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="261" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>415</v>
       </c>
@@ -14237,7 +14237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="262" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>417</v>
       </c>
@@ -14281,7 +14281,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="263" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>418</v>
       </c>
@@ -14325,7 +14325,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="264" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>419</v>
       </c>
@@ -14372,7 +14372,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="265" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>421</v>
       </c>
@@ -14419,7 +14419,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="266" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>423</v>
       </c>
@@ -14466,7 +14466,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="267" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>425</v>
       </c>
@@ -14513,7 +14513,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="268" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>427</v>
       </c>
@@ -14560,7 +14560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="269" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>429</v>
       </c>
@@ -14607,7 +14607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="270" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>431</v>
       </c>
@@ -14654,7 +14654,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="271" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>433</v>
       </c>
@@ -14742,7 +14742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="273" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>435</v>
       </c>
@@ -14830,7 +14830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="275" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>437</v>
       </c>
@@ -14874,7 +14874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="276" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>438</v>
       </c>
@@ -14921,7 +14921,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="277" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>439</v>
       </c>
@@ -14965,7 +14965,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="278" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>440</v>
       </c>
@@ -15012,7 +15012,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="279" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>442</v>
       </c>
@@ -15056,7 +15056,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="280" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>443</v>
       </c>
@@ -15103,7 +15103,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="281" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>445</v>
       </c>
@@ -15147,7 +15147,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="282" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>446</v>
       </c>
@@ -15191,7 +15191,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="283" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>447</v>
       </c>
@@ -15235,7 +15235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="284" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>448</v>
       </c>
@@ -15279,7 +15279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="285" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>449</v>
       </c>
@@ -15326,7 +15326,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="286" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>451</v>
       </c>
@@ -15373,7 +15373,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="287" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>453</v>
       </c>
@@ -15420,7 +15420,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="288" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>455</v>
       </c>
@@ -15464,7 +15464,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="289" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>456</v>
       </c>
@@ -15508,7 +15508,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="290" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>457</v>
       </c>
@@ -15599,7 +15599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="292" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>460</v>
       </c>
@@ -15646,7 +15646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="293" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>462</v>
       </c>
@@ -15690,7 +15690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="294" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>463</v>
       </c>
@@ -15737,7 +15737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="295" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>465</v>
       </c>
@@ -15781,7 +15781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="296" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>466</v>
       </c>
@@ -15869,7 +15869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="298" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>468</v>
       </c>
@@ -15916,7 +15916,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="299" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>470</v>
       </c>
@@ -16001,7 +16001,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="301" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>472</v>
       </c>
@@ -16092,7 +16092,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="303" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>475</v>
       </c>
@@ -16139,7 +16139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="304" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>477</v>
       </c>
@@ -16183,7 +16183,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="305" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>478</v>
       </c>
@@ -16227,7 +16227,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="306" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>479</v>
       </c>
@@ -16274,7 +16274,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="307" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>481</v>
       </c>
@@ -16318,7 +16318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="308" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>482</v>
       </c>
@@ -16362,7 +16362,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="309" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>483</v>
       </c>
@@ -16409,7 +16409,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="310" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>485</v>
       </c>
@@ -16497,7 +16497,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="312" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>487</v>
       </c>
@@ -16544,7 +16544,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="313" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>489</v>
       </c>
@@ -16588,7 +16588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="314" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>490</v>
       </c>
@@ -16682,7 +16682,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="316" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>494</v>
       </c>
@@ -16726,7 +16726,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="317" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>495</v>
       </c>
@@ -16858,7 +16858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="320" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>498</v>
       </c>
@@ -16902,7 +16902,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="321" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>499</v>
       </c>
@@ -16946,7 +16946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="322" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>500</v>
       </c>
@@ -16990,7 +16990,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="323" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>501</v>
       </c>
@@ -17081,7 +17081,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="325" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>504</v>
       </c>
@@ -17128,7 +17128,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="326" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>506</v>
       </c>
@@ -17172,7 +17172,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="327" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>507</v>
       </c>
@@ -17219,7 +17219,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="328" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>509</v>
       </c>
@@ -17266,7 +17266,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="329" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>511</v>
       </c>
@@ -17313,7 +17313,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="330" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>513</v>
       </c>
@@ -17360,7 +17360,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="331" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>515</v>
       </c>
@@ -17451,7 +17451,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="333" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>518</v>
       </c>
@@ -17498,7 +17498,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="334" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>520</v>
       </c>
@@ -17592,7 +17592,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="336" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>524</v>
       </c>
@@ -17683,7 +17683,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="338" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>527</v>
       </c>
@@ -17730,7 +17730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="339" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>529</v>
       </c>
@@ -17774,7 +17774,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="340" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>530</v>
       </c>
@@ -17818,7 +17818,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="341" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>531</v>
       </c>
@@ -17862,7 +17862,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="342" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>532</v>
       </c>
@@ -17953,7 +17953,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="344" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>535</v>
       </c>
@@ -17997,7 +17997,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="345" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>536</v>
       </c>
@@ -18044,7 +18044,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="346" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>538</v>
       </c>
@@ -18226,7 +18226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="350" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>544</v>
       </c>
@@ -18273,7 +18273,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="351" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>546</v>
       </c>
@@ -18367,7 +18367,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="353" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>550</v>
       </c>
@@ -18414,7 +18414,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="354" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>552</v>
       </c>
@@ -18458,7 +18458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="355" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>553</v>
       </c>
@@ -18505,7 +18505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="356" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>555</v>
       </c>
@@ -18552,7 +18552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="357" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>557</v>
       </c>
@@ -18787,7 +18787,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="362" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>567</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="364" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>570</v>
       </c>
@@ -18922,7 +18922,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="365" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>571</v>
       </c>
@@ -18966,7 +18966,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="366" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>572</v>
       </c>
@@ -19010,7 +19010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="367" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>573</v>
       </c>
@@ -19054,7 +19054,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="368" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>574</v>
       </c>
@@ -19101,7 +19101,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="369" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>576</v>
       </c>
@@ -19192,7 +19192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="371" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>579</v>
       </c>
@@ -19236,7 +19236,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="372" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>580</v>
       </c>
@@ -19280,7 +19280,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="373" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>581</v>
       </c>
@@ -19324,7 +19324,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="374" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>582</v>
       </c>
@@ -19368,7 +19368,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="375" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>583</v>
       </c>
@@ -19415,7 +19415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="376" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>585</v>
       </c>
@@ -19462,7 +19462,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="377" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>587</v>
       </c>
@@ -19509,7 +19509,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="378" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>589</v>
       </c>
@@ -19556,7 +19556,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="379" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>591</v>
       </c>
@@ -19603,7 +19603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="380" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>593</v>
       </c>
@@ -19647,7 +19647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="381" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>594</v>
       </c>
@@ -19691,7 +19691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="382" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>595</v>
       </c>
@@ -19735,7 +19735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="383" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>596</v>
       </c>
@@ -19782,7 +19782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="384" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>598</v>
       </c>
@@ -19826,7 +19826,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="385" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>599</v>
       </c>
@@ -19967,7 +19967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="388" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>605</v>
       </c>
@@ -20011,7 +20011,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="389" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>606</v>
       </c>
@@ -20055,7 +20055,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="390" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>607</v>
       </c>
@@ -20102,7 +20102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="391" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>609</v>
       </c>
@@ -20146,7 +20146,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="392" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>610</v>
       </c>
@@ -20237,7 +20237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="394" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>613</v>
       </c>
@@ -20281,7 +20281,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="395" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>614</v>
       </c>
@@ -20375,7 +20375,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="397" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>618</v>
       </c>
@@ -20422,7 +20422,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="398" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>620</v>
       </c>
@@ -20516,7 +20516,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="400" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>624</v>
       </c>
@@ -20563,7 +20563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="401" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>626</v>
       </c>
@@ -20607,7 +20607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="402" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>627</v>
       </c>
@@ -20701,7 +20701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="404" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>631</v>
       </c>
@@ -20748,7 +20748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="405" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>633</v>
       </c>
@@ -20795,7 +20795,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="406" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>635</v>
       </c>
@@ -20841,11 +20841,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O406" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="CPTS11"/>
-      </filters>
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="lessThanOrEqual" val="1"/>
+      </customFilters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O406">
+      <sortCondition ref="A1:A406"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>